<commit_message>
Started on flavors page
</commit_message>
<xml_diff>
--- a/public/flavors.xlsx
+++ b/public/flavors.xlsx
@@ -1038,9 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Added buttons to flavors page
</commit_message>
<xml_diff>
--- a/public/flavors.xlsx
+++ b/public/flavors.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Classic" sheetId="1" r:id="rId1"/>
     <sheet name="Gourmet" sheetId="2" r:id="rId2"/>
     <sheet name="Icings" sheetId="3" r:id="rId3"/>
     <sheet name="Fillings" sheetId="4" r:id="rId4"/>
-    <sheet name="Gluten-Free Options" sheetId="5" r:id="rId5"/>
+    <sheet name="Gluten-Free" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1038,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1364,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>